<commit_message>
Update: sửa lại quote 6)
</commit_message>
<xml_diff>
--- a/WIP/Users/HaiCM/Yêu cầu slider image.xlsx
+++ b/WIP/Users/HaiCM/Yêu cầu slider image.xlsx
@@ -57,9 +57,6 @@
     <t>5) Một người thích đọc sẽ sống cả ngàn năm trước khi chết</t>
   </si>
   <si>
-    <t>6) Một cuốn sách tuyệt vời mà bạn đọc có thể mang đến những điều diệu kỳ</t>
-  </si>
-  <si>
     <t>Số lượng 10 cái</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t xml:space="preserve"> Emma Gulliford</t>
   </si>
   <si>
-    <t xml:space="preserve"> J. K. Jowling</t>
-  </si>
-  <si>
     <t xml:space="preserve"> George R.R Martin</t>
   </si>
   <si>
@@ -113,6 +107,12 @@
   </si>
   <si>
     <t>Designer có quyền làm theo những gì hợp lí. Ngoại trừ viện thay đổi vị trí form thì những việc khác như quote khác hay hơn, phương án xử lí về việc form tốt hơn đều chấp nhận.</t>
+  </si>
+  <si>
+    <t>6) Bạn biết rằng bạn đã đọc một cuốn sách hay khi bạn giở đến trang cuối cùng và cảm thấy như mình vừa chia tay một người bạn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul Sweeney</t>
   </si>
 </sst>
 </file>
@@ -303,6 +303,45 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -318,18 +357,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -338,33 +365,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,7 +738,7 @@
   <dimension ref="C4:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E16" sqref="E16:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,16 +753,16 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:10" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="3:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
@@ -771,14 +771,14 @@
       <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
     </row>
     <row r="6" spans="3:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
@@ -787,252 +787,237 @@
       <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="24"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <v>2</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
+      <c r="E7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="3:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <v>3</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="13" t="s">
+      <c r="D8" s="23"/>
+      <c r="E8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="27"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="3:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <v>4</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="21" t="s">
+      <c r="D9" s="23"/>
+      <c r="E9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="20"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="19"/>
     </row>
     <row r="10" spans="3:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <v>5</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="21" t="s">
+      <c r="D10" s="23"/>
+      <c r="E10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="20"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="19"/>
     </row>
     <row r="11" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <v>6</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="21" t="s">
+      <c r="D11" s="23"/>
+      <c r="E11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="20"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="19"/>
     </row>
     <row r="12" spans="3:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <v>7</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="21" t="s">
+      <c r="D12" s="23"/>
+      <c r="E12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="20"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="19"/>
     </row>
     <row r="13" spans="3:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <v>8</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="20"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="19"/>
     </row>
     <row r="14" spans="3:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <v>9</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14" s="20"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="19"/>
     </row>
     <row r="15" spans="3:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <v>10</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="15"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" spans="3:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <v>11</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="15"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="8"/>
     </row>
     <row r="17" spans="3:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <v>12</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="17"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="3:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <v>13</v>
       </c>
       <c r="D18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="19" spans="3:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <v>14</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
+      <c r="D19" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
     </row>
     <row r="22" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
     <mergeCell ref="D22:E24"/>
     <mergeCell ref="E18:J18"/>
     <mergeCell ref="D19:J19"/>
@@ -1049,6 +1034,21 @@
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="E15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>